<commit_message>
Adding loading of already made queries.
</commit_message>
<xml_diff>
--- a/Example/Filled/AR1 - Q2.2023.xlsx
+++ b/Example/Filled/AR1 - Q2.2023.xlsx
@@ -2303,7 +2303,7 @@
         </is>
       </c>
       <c r="F22" s="136" t="n">
-        <v>2235</v>
+        <v>2246</v>
       </c>
       <c r="G22" s="136" t="inlineStr"/>
     </row>
@@ -11111,24 +11111,12 @@
           <t>Namibia</t>
         </is>
       </c>
-      <c r="D115" s="140" t="n">
-        <v>8079</v>
-      </c>
-      <c r="E115" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="F115" s="140" t="n">
-        <v>0</v>
-      </c>
-      <c r="G115" s="138" t="n">
-        <v>775078.85</v>
-      </c>
-      <c r="H115" s="138" t="n">
-        <v>0</v>
-      </c>
-      <c r="I115" s="139" t="n">
-        <v>0</v>
-      </c>
+      <c r="D115" s="140" t="inlineStr"/>
+      <c r="E115" s="140" t="inlineStr"/>
+      <c r="F115" s="140" t="inlineStr"/>
+      <c r="G115" s="138" t="inlineStr"/>
+      <c r="H115" s="138" t="inlineStr"/>
+      <c r="I115" s="139" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" s="153" t="inlineStr">

</xml_diff>

<commit_message>
Making changes for AR2 and AR1 according to NBP errors.
</commit_message>
<xml_diff>
--- a/Example/Filled/AR1 - Q2.2023.xlsx
+++ b/Example/Filled/AR1 - Q2.2023.xlsx
@@ -2303,7 +2303,7 @@
         </is>
       </c>
       <c r="F22" s="136" t="n">
-        <v>2288</v>
+        <v>2425</v>
       </c>
       <c r="G22" s="136" t="inlineStr"/>
     </row>
@@ -13557,7 +13557,7 @@
         <v>3586.97</v>
       </c>
       <c r="J10" s="153" t="n">
-        <v>9344.23</v>
+        <v>11670.23</v>
       </c>
       <c r="K10" s="41" t="n"/>
     </row>
@@ -13594,7 +13594,7 @@
         <v>3586.97</v>
       </c>
       <c r="J11" s="153" t="n">
-        <v>9344.23</v>
+        <v>11670.23</v>
       </c>
       <c r="K11" s="41" t="n"/>
     </row>
@@ -13739,7 +13739,7 @@
         <v>3586.97</v>
       </c>
       <c r="J15" s="153" t="n">
-        <v>9344.23</v>
+        <v>11670.23</v>
       </c>
       <c r="K15" s="41" t="n"/>
     </row>
@@ -14390,37 +14390,37 @@
       </c>
       <c r="C11" s="149" t="inlineStr">
         <is>
-          <t>+48 506 297 621</t>
+          <t>8</t>
         </is>
       </c>
       <c r="D11" s="149" t="inlineStr">
         <is>
-          <t>+48 506 297 621</t>
+          <t>8</t>
         </is>
       </c>
       <c r="E11" s="149" t="inlineStr">
         <is>
-          <t>+48 506 297 621</t>
+          <t>8</t>
         </is>
       </c>
       <c r="F11" s="149" t="inlineStr">
         <is>
-          <t>+48 506 297 621</t>
+          <t>8</t>
         </is>
       </c>
       <c r="G11" s="149" t="inlineStr">
         <is>
-          <t>+48 506 297 621</t>
+          <t>8</t>
         </is>
       </c>
       <c r="H11" s="149" t="inlineStr">
         <is>
-          <t>+48 506 297 621</t>
+          <t>8</t>
         </is>
       </c>
       <c r="I11" s="149" t="inlineStr">
         <is>
-          <t>+48 506 297 621</t>
+          <t>8</t>
         </is>
       </c>
     </row>
@@ -14437,37 +14437,37 @@
       </c>
       <c r="C12" s="148" t="inlineStr">
         <is>
-          <t>krzysztof.kaniewski@paytel.pl</t>
+          <t>k</t>
         </is>
       </c>
       <c r="D12" s="148" t="inlineStr">
         <is>
-          <t>krzysztof.kaniewski@paytel.pl</t>
+          <t>k</t>
         </is>
       </c>
       <c r="E12" s="148" t="inlineStr">
         <is>
-          <t>krzysztof.kaniewski@paytel.pl</t>
+          <t>k</t>
         </is>
       </c>
       <c r="F12" s="148" t="inlineStr">
         <is>
-          <t>krzysztof.kaniewski@paytel.pl</t>
+          <t>k</t>
         </is>
       </c>
       <c r="G12" s="148" t="inlineStr">
         <is>
-          <t>krzysztof.kaniewski@paytel.pl</t>
+          <t>k</t>
         </is>
       </c>
       <c r="H12" s="148" t="inlineStr">
         <is>
-          <t>krzysztof.kaniewski@paytel.pl</t>
+          <t>k</t>
         </is>
       </c>
       <c r="I12" s="148" t="inlineStr">
         <is>
-          <t>krzysztof.kaniewski@paytel.pl</t>
+          <t>k</t>
         </is>
       </c>
     </row>

</xml_diff>